<commit_message>
Update bugs and robustness
</commit_message>
<xml_diff>
--- a/vft_config.xlsx
+++ b/vft_config.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14787617-81B9-4652-A39C-EE1C66A42034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7D2FDB-9C8A-4A4A-9FB1-5E1156ED25FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-25740" yWindow="1725" windowWidth="21600" windowHeight="11295" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
-    <sheet name="units_sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
     <sheet name="data_sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -477,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -577,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B33013-4172-2E43-B04F-F034BA65B290}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>